<commit_message>
Created Streamiing 0 Done
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Parallel-Computing-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965C2181-3DD2-4047-BE4F-AB0C972D0D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6BBB9B-AE89-4921-819E-C764469310EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>gpu_3.cu</t>
   </si>
@@ -188,6 +188,36 @@
   </si>
   <si>
     <t>4.7670us</t>
+  </si>
+  <si>
+    <t>Stream version(0)</t>
+  </si>
+  <si>
+    <t>gpu_3_stream_0.cu</t>
+  </si>
+  <si>
+    <t>297.30us</t>
+  </si>
+  <si>
+    <t>4.1622ms</t>
+  </si>
+  <si>
+    <t>2.1937ms</t>
+  </si>
+  <si>
+    <t>48.749us</t>
+  </si>
+  <si>
+    <t>665.29us</t>
+  </si>
+  <si>
+    <t>14.462us</t>
+  </si>
+  <si>
+    <t>9.5370us</t>
+  </si>
+  <si>
+    <t>Streamed copy of datapoints at the first with K2 then begin iteratoions with K2 :D</t>
   </si>
 </sst>
 </file>
@@ -209,7 +239,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +282,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -502,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -564,15 +600,27 @@
     <xf numFmtId="10" fontId="1" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="1" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -582,16 +630,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -874,11 +913,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J38" sqref="J38"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -900,153 +939,187 @@
     <col min="15" max="15" width="14.08984375" customWidth="1"/>
     <col min="16" max="16" width="14.81640625" customWidth="1"/>
     <col min="17" max="17" width="19.54296875" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="19" max="19" width="14.08984375" customWidth="1"/>
+    <col min="20" max="20" width="14.81640625" customWidth="1"/>
+    <col min="21" max="21" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:17" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="22" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="21" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="22" t="s">
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="23"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="26"/>
     </row>
-    <row r="3" spans="1:17" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="27" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="27" t="s">
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="29"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="24"/>
     </row>
-    <row r="4" spans="1:17" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="27" t="s">
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="27" t="s">
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="29"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="24"/>
     </row>
-    <row r="5" spans="1:17" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="28">
         <v>10</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27">
-        <v>14</v>
-      </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="27">
-        <v>14</v>
-      </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="27">
-        <v>14</v>
-      </c>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="22">
+        <v>14</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="22">
+        <v>14</v>
+      </c>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="22">
+        <v>14</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="22">
+        <v>14</v>
+      </c>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="24"/>
     </row>
-    <row r="6" spans="1:17" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="28">
         <v>0.32800000000000001</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27">
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="22">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="27">
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="22">
         <v>0.04</v>
       </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="27">
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="22">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="29"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="24"/>
     </row>
-    <row r="7" spans="1:17" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -1088,8 +1161,20 @@
       <c r="Q7" s="11" t="s">
         <v>13</v>
       </c>
+      <c r="R7" s="10">
+        <v>3</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -1133,8 +1218,20 @@
       <c r="Q8" s="20" t="s">
         <v>33</v>
       </c>
+      <c r="R8" s="12">
+        <v>0.57469999999999999</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="T8" s="1">
+        <v>14</v>
+      </c>
+      <c r="U8" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -1163,7 +1260,7 @@
       <c r="L9" s="1">
         <v>14</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="21" t="s">
         <v>22</v>
       </c>
       <c r="N9" s="12">
@@ -1178,8 +1275,20 @@
       <c r="Q9" s="13" t="s">
         <v>35</v>
       </c>
+      <c r="R9" s="12">
+        <v>0.3029</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="T9" s="1">
+        <v>45</v>
+      </c>
+      <c r="U9" s="31" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -1223,8 +1332,20 @@
       <c r="Q10" s="13" t="s">
         <v>38</v>
       </c>
+      <c r="R10" s="12">
+        <v>9.1899999999999996E-2</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" s="1">
+        <v>46</v>
+      </c>
+      <c r="U10" s="31" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
@@ -1268,8 +1389,20 @@
       <c r="Q11" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="R11" s="12">
+        <v>2.93E-2</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="T11" s="1">
+        <v>29</v>
+      </c>
+      <c r="U11" s="13" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:21" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="19" t="s">
         <v>27</v>
       </c>
@@ -1301,8 +1434,8 @@
       <c r="M12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="N12" s="14" t="s">
-        <v>41</v>
+      <c r="N12" s="14">
+        <v>1.5E-3</v>
       </c>
       <c r="O12" s="8" t="s">
         <v>42</v>
@@ -1313,9 +1446,31 @@
       <c r="Q12" s="15" t="s">
         <v>41</v>
       </c>
+      <c r="R12" s="14">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="T12" s="8">
+        <v>28</v>
+      </c>
+      <c r="U12" s="15" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="25">
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -1331,11 +1486,6 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Shilloute to CPU
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Parallel-Computing-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6BBB9B-AE89-4921-819E-C764469310EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90334B24-C43D-4DAB-A76F-0AF78E03DBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -603,6 +603,15 @@
     <xf numFmtId="10" fontId="1" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="1" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -612,12 +621,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -628,9 +631,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -950,174 +950,174 @@
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="25" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="27" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="25" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="25" t="s">
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="26"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="24"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="22" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="22" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="22" t="s">
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="22" t="s">
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="24"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="27"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="22" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="22" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="22" t="s">
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="22" t="s">
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="24"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="27"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="29">
         <v>10</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="22">
-        <v>14</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="22">
-        <v>14</v>
-      </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="22">
-        <v>14</v>
-      </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="22">
-        <v>14</v>
-      </c>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="24"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="25">
+        <v>14</v>
+      </c>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="25">
+        <v>14</v>
+      </c>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="25">
+        <v>14</v>
+      </c>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="25">
+        <v>14</v>
+      </c>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="27"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="29">
         <v>0.32800000000000001</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="22">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="25">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="22">
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="25">
         <v>0.04</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="22">
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="25">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="22">
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="25">
         <v>0.05</v>
       </c>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="24"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="27"/>
     </row>
     <row r="7" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
@@ -1284,7 +1284,7 @@
       <c r="T9" s="1">
         <v>45</v>
       </c>
-      <c r="U9" s="31" t="s">
+      <c r="U9" s="22" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       <c r="T10" s="1">
         <v>46</v>
       </c>
-      <c r="U10" s="31" t="s">
+      <c r="U10" s="22" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1461,16 +1461,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -1486,6 +1476,16 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Reduction Sum to K3
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Parallel-Computing-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1221F7-1DDB-4F1F-85F8-53C69C58595A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9B5471-4125-41FE-82DB-B9D1E407D078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,8 +36,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dell</author>
+  </authors>
+  <commentList>
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{06ACA96D-5C49-4803-9B79-EF3B41A78A99}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Arguments per blocks
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M14" authorId="0" shapeId="0" xr:uid="{E482D505-9C4D-420A-91F7-76A3920C9F1E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+bec we copy only result at 0 not al scores by blocks</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
   <si>
     <t>gpu_3.cu</t>
   </si>
@@ -290,13 +349,64 @@
   </si>
   <si>
     <t>Seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GPU version(1) Stream (1)</t>
+  </si>
+  <si>
+    <t>Added Atomic Add to score in K3</t>
+  </si>
+  <si>
+    <t>1.82168s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.82168s </t>
+  </si>
+  <si>
+    <t>4.9742ms</t>
+  </si>
+  <si>
+    <t>382.63us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42.115us </t>
+  </si>
+  <si>
+    <t>8.4880us</t>
+  </si>
+  <si>
+    <t>26 1.0560us</t>
+  </si>
+  <si>
+    <t>1.8531ms</t>
+  </si>
+  <si>
+    <t>381.98us</t>
+  </si>
+  <si>
+    <t>136.96us</t>
+  </si>
+  <si>
+    <t>27.456us</t>
+  </si>
+  <si>
+    <t>1.83433s</t>
+  </si>
+  <si>
+    <t>1.82353s</t>
+  </si>
+  <si>
+    <t>Cancalled back to v0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.8910us </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,8 +426,32 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +500,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -629,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -700,21 +840,30 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -727,13 +876,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1053,174 +1205,174 @@
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="24" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="29" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="24" t="s">
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="24" t="s">
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="25"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="31"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="26" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="26" t="s">
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="26" t="s">
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="26" t="s">
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="29"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="26" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="26" t="s">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="26" t="s">
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="26" t="s">
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="29"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="33">
         <v>10</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="26">
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="27">
         <v>14</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="26">
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="27">
         <v>14</v>
       </c>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="26">
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="27">
         <v>14</v>
       </c>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="26">
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="27">
         <v>14</v>
       </c>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="29"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="33">
         <v>0.32800000000000001</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="26">
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="27">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="26">
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="27">
         <v>0.04</v>
       </c>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="26">
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="27">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="26">
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="27">
         <v>0.05</v>
       </c>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="29"/>
     </row>
     <row r="7" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
@@ -1564,6 +1716,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -1579,28 +1741,18 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6EC81A-94A0-466F-8869-78A7FD8B6882}">
-  <dimension ref="A1:U16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6EC81A-94A0-466F-8869-78A7FD8B6882}">
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1633,190 +1785,204 @@
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="24" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="25"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="31"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="26" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="29"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="28"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="29"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="26">
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="27">
         <v>42</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
-      <c r="U5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="27">
+        <v>42</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="29"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="26">
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="27">
         <v>13</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="27">
+        <v>13</v>
+      </c>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="29"/>
     </row>
     <row r="7" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="26">
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="27">
         <v>0.61830700000000005</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="27">
+        <v>0.61830700000000005</v>
+      </c>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="29"/>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="26" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="27">
+        <v>1.8245990000000001</v>
+      </c>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="29"/>
     </row>
     <row r="9" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
@@ -1893,10 +2059,18 @@
       <c r="I10" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="13"/>
+      <c r="J10" s="12">
+        <v>0.996</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10" s="37" t="s">
+        <v>87</v>
+      </c>
       <c r="N10" s="12"/>
       <c r="O10" s="6"/>
       <c r="P10" s="1"/>
@@ -1926,10 +2100,18 @@
       <c r="I11" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="13"/>
+      <c r="J11" s="12">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" s="1">
+        <v>13</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="N11" s="12"/>
       <c r="O11" s="6"/>
       <c r="P11" s="1"/>
@@ -1959,10 +2141,18 @@
       <c r="I12" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="13"/>
+      <c r="J12" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="L12" s="1">
+        <v>44</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>90</v>
+      </c>
       <c r="N12" s="12"/>
       <c r="O12" s="6"/>
       <c r="P12" s="1"/>
@@ -1992,10 +2182,18 @@
       <c r="I13" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="13"/>
+      <c r="J13" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="1">
+        <v>45</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="N13" s="12"/>
       <c r="O13" s="6"/>
       <c r="P13" s="1"/>
@@ -2025,10 +2223,18 @@
       <c r="I14" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="13"/>
+      <c r="J14" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" s="1">
+        <v>28</v>
+      </c>
+      <c r="M14" s="39" t="s">
+        <v>100</v>
+      </c>
       <c r="N14" s="12"/>
       <c r="O14" s="6"/>
       <c r="P14" s="1"/>
@@ -2058,10 +2264,18 @@
       <c r="I15" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="15"/>
+      <c r="J15" s="14">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15" s="8">
+        <v>26</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="N15" s="14"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
@@ -2072,56 +2286,90 @@
       <c r="U15" s="15"/>
     </row>
     <row r="16" spans="1:21" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F16" s="33">
+      <c r="F16" s="24">
         <f>SUM(F10:F15)</f>
         <v>0.99990000000000001</v>
       </c>
-      <c r="G16" s="34" t="s">
+      <c r="G16" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="H16" s="35"/>
-      <c r="I16" s="34" t="s">
+      <c r="H16" s="26"/>
+      <c r="I16" s="25" t="s">
         <v>80</v>
       </c>
+      <c r="J16" s="24">
+        <f>SUM(J10:J15)</f>
+        <v>1</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="L16" s="26"/>
+      <c r="M16" s="36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="J18" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+    </row>
+    <row r="19" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+    </row>
+    <row r="20" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="36">
+    <mergeCell ref="J18:M20"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="R6:U6"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="R5:U5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="R8:U8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 3 and 4 to be completed
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Parallel-Computing-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9B5471-4125-41FE-82DB-B9D1E407D078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B396C10-A862-48A4-9327-056B064EFF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
   <si>
     <t>gpu_3.cu</t>
   </si>
@@ -400,6 +400,15 @@
   </si>
   <si>
     <t xml:space="preserve">4.8910us </t>
+  </si>
+  <si>
+    <t>gpu_3_stream_0_sihouette_1.cu</t>
+  </si>
+  <si>
+    <t>gpu_3_stream_0_sihouette_2.cu</t>
+  </si>
+  <si>
+    <t>Reduction Sum K3</t>
   </si>
 </sst>
 </file>
@@ -849,6 +858,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -858,12 +882,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -874,19 +892,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1205,7 +1214,7 @@
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="30"/>
@@ -1217,7 +1226,7 @@
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
       <c r="I2" s="31"/>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="35" t="s">
         <v>16</v>
       </c>
       <c r="K2" s="30"/>
@@ -1240,139 +1249,139 @@
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="27" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="27" t="s">
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="27" t="s">
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="27" t="s">
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="29"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="34"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="27" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="27" t="s">
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="27" t="s">
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="27" t="s">
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="29"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="34"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="36">
         <v>10</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="27">
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="32">
         <v>14</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="27">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="32">
         <v>14</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="27">
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="32">
         <v>14</v>
       </c>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="27">
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="32">
         <v>14</v>
       </c>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="29"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="34"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="36">
         <v>0.32800000000000001</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="27">
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="32">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="27">
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="32">
         <v>0.04</v>
       </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="27">
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="32">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="27">
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="32">
         <v>0.05</v>
       </c>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="29"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="34"/>
     </row>
     <row r="7" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
@@ -1716,16 +1725,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -1741,6 +1740,16 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1750,9 +1759,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6EC81A-94A0-466F-8869-78A7FD8B6882}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1785,7 +1794,7 @@
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="30"/>
@@ -1816,173 +1825,177 @@
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="27" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="29"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="34"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="27" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="29"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="34"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="27">
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="32">
         <v>42</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="27">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="32">
         <v>42</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="29"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="34"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="27">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="32">
         <v>13</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="27">
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="32">
         <v>13</v>
       </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="29"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="34"/>
     </row>
     <row r="7" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="27">
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="32">
         <v>0.61830700000000005</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="27">
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="32">
         <v>0.61830700000000005</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="29"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="34"/>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="27" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="27">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="32">
         <v>1.8245990000000001</v>
       </c>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28"/>
-      <c r="U8" s="29"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="34"/>
     </row>
     <row r="9" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
@@ -2068,7 +2081,7 @@
       <c r="L10" s="1">
         <v>1</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="M10" s="28" t="s">
         <v>87</v>
       </c>
       <c r="N10" s="12"/>
@@ -2232,7 +2245,7 @@
       <c r="L14" s="1">
         <v>28</v>
       </c>
-      <c r="M14" s="39" t="s">
+      <c r="M14" s="29" t="s">
         <v>100</v>
       </c>
       <c r="N14" s="12"/>
@@ -2305,37 +2318,47 @@
         <v>97</v>
       </c>
       <c r="L16" s="26"/>
-      <c r="M16" s="36" t="s">
+      <c r="M16" s="27" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="18" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J18" s="38" t="s">
+      <c r="J18" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
     </row>
     <row r="19" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
     </row>
     <row r="20" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="J18:M20"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
     <mergeCell ref="R8:U8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:I4"/>
@@ -2347,26 +2370,16 @@
     <mergeCell ref="J7:M7"/>
     <mergeCell ref="N7:Q7"/>
     <mergeCell ref="R7:U7"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R3:U3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="R6:U6"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="J18:M20"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Tiling to K3 for computation
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Parallel-Computing-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B396C10-A862-48A4-9327-056B064EFF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF986FED-C0AA-4ECE-AEB1-F9D518D056E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="106">
   <si>
     <t>gpu_3.cu</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Reduction Sum K3</t>
+  </si>
+  <si>
+    <t>gpu_3_stream_0_sihouette_2_mul.cu</t>
+  </si>
+  <si>
+    <t>Added Tiling to K3  Tile Dim 128 Thread per block 32</t>
   </si>
 </sst>
 </file>
@@ -867,19 +873,19 @@
     <xf numFmtId="10" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1217,33 +1223,33 @@
       <c r="B2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="30" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="31"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="30" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="30" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="31"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
@@ -1255,30 +1261,30 @@
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="32" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="32" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="32" t="s">
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="34"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
@@ -1288,30 +1294,30 @@
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
       <c r="E4" s="38"/>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="32" t="s">
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="32" t="s">
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="32" t="s">
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="34"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="32"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
@@ -1323,30 +1329,30 @@
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
       <c r="E5" s="38"/>
-      <c r="F5" s="32">
+      <c r="F5" s="30">
         <v>14</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="32">
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="30">
         <v>14</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="32">
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="30">
         <v>14</v>
       </c>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="32">
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="30">
         <v>14</v>
       </c>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="34"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="32"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
@@ -1358,30 +1364,30 @@
       <c r="C6" s="37"/>
       <c r="D6" s="37"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="32">
+      <c r="F6" s="30">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="32">
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="30">
         <v>0.04</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="32">
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="30">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="32">
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="30">
         <v>0.05</v>
       </c>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="34"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="32"/>
     </row>
     <row r="7" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
@@ -1725,6 +1731,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -1740,16 +1756,6 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1760,8 +1766,8 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P15" sqref="P15"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R5" sqref="R5:U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1797,29 +1803,29 @@
       <c r="B2" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="30" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="30" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="31"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
@@ -1829,28 +1835,30 @@
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="32" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="32" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="34"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
@@ -1860,113 +1868,115 @@
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
       <c r="E4" s="38"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="32" t="s">
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="32" t="s">
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="34"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="32"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="32">
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="30">
         <v>42</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="32">
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="30">
         <v>42</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="34"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="32"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="32">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="30">
         <v>13</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="32">
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="30">
         <v>13</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="34"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="32"/>
     </row>
     <row r="7" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="32">
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="30">
         <v>0.61830700000000005</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="32">
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="30">
         <v>0.61830700000000005</v>
       </c>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33"/>
-      <c r="U7" s="34"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="32"/>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
@@ -1976,26 +1986,26 @@
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
       <c r="E8" s="38"/>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="32">
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="30">
         <v>1.8245990000000001</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="34"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="32"/>
     </row>
     <row r="9" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
@@ -2344,21 +2354,11 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="J18:M20"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
     <mergeCell ref="R8:U8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:I4"/>
@@ -2375,11 +2375,21 @@
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="R6:U6"/>
-    <mergeCell ref="J18:M20"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Sum for block
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Parallel-Computing-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF986FED-C0AA-4ECE-AEB1-F9D518D056E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C74BFD7-238D-4D3E-A14F-61CF64BC19EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
   <si>
     <t>gpu_3.cu</t>
   </si>
@@ -415,6 +415,90 @@
   </si>
   <si>
     <t>Added Tiling to K3  Tile Dim 128 Thread per block 32</t>
+  </si>
+  <si>
+    <t>1.92609s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.92609s </t>
+  </si>
+  <si>
+    <t>383.67us</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.9877ms</t>
+  </si>
+  <si>
+    <t>42.108us</t>
+  </si>
+  <si>
+    <t>1.8528ms</t>
+  </si>
+  <si>
+    <t>8.4440us</t>
+  </si>
+  <si>
+    <t>380.00us</t>
+  </si>
+  <si>
+    <t>8.5050us</t>
+  </si>
+  <si>
+    <t>238.15us</t>
+  </si>
+  <si>
+    <t>26.336us</t>
+  </si>
+  <si>
+    <t>1.0120us</t>
+  </si>
+  <si>
+    <t>1.931982 sec</t>
+  </si>
+  <si>
+    <t>1.827291 sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.65274s </t>
+  </si>
+  <si>
+    <t>1.65274s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 214.39us</t>
+  </si>
+  <si>
+    <t>2.7870ms</t>
+  </si>
+  <si>
+    <t>16.388us</t>
+  </si>
+  <si>
+    <t>721.10us</t>
+  </si>
+  <si>
+    <t>8.0630us</t>
+  </si>
+  <si>
+    <t>362.84us</t>
+  </si>
+  <si>
+    <t>4.7500us</t>
+  </si>
+  <si>
+    <t>133.02us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">612ns </t>
+  </si>
+  <si>
+    <t>15.935us</t>
+  </si>
+  <si>
+    <t>1.65675s</t>
+  </si>
+  <si>
+    <t>1.652984s</t>
   </si>
 </sst>
 </file>
@@ -873,6 +957,12 @@
     <xf numFmtId="10" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -880,12 +970,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1223,33 +1307,33 @@
       <c r="B2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="33" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
       <c r="J2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="33" t="s">
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="33" t="s">
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="34"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="31"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
@@ -1261,30 +1345,30 @@
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30" t="s">
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="30" t="s">
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="30" t="s">
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="32"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="34"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
@@ -1294,30 +1378,30 @@
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
       <c r="E4" s="38"/>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="30" t="s">
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="30" t="s">
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="32"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="34"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
@@ -1329,30 +1413,30 @@
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
       <c r="E5" s="38"/>
-      <c r="F5" s="30">
+      <c r="F5" s="32">
         <v>14</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="30">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="32">
         <v>14</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="30">
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="32">
         <v>14</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="30">
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="32">
         <v>14</v>
       </c>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="32"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="34"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
@@ -1364,30 +1448,30 @@
       <c r="C6" s="37"/>
       <c r="D6" s="37"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="30">
+      <c r="F6" s="32">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="30">
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="32">
         <v>0.04</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="30">
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="32">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="30">
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="32">
         <v>0.05</v>
       </c>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="32"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="34"/>
     </row>
     <row r="7" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
@@ -1731,16 +1815,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -1756,6 +1830,16 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1765,9 +1849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6EC81A-94A0-466F-8869-78A7FD8B6882}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R5" sqref="R5:U5"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1803,29 +1887,29 @@
       <c r="B2" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="33" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="33" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="34"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="31"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
@@ -1835,30 +1919,30 @@
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30" t="s">
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="30" t="s">
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="30" t="s">
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="32"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="34"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
@@ -1868,115 +1952,127 @@
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
       <c r="E4" s="38"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="30" t="s">
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="30" t="s">
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="32"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="34"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30">
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="32">
         <v>42</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="30">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="32">
         <v>42</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="32"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="32">
+        <v>42</v>
+      </c>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="32">
+        <v>42</v>
+      </c>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="34"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30">
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="32">
         <v>13</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="30">
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="32">
         <v>13</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="32"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="32">
+        <v>32</v>
+      </c>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="32">
+        <v>13</v>
+      </c>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="34"/>
     </row>
     <row r="7" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="30">
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="32">
         <v>0.61830700000000005</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="30">
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="32">
         <v>0.61830700000000005</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="32"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="32">
+        <v>0.61830700000000005</v>
+      </c>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="32">
+        <v>0.61830700000000005</v>
+      </c>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="34"/>
     </row>
     <row r="8" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
@@ -1986,26 +2082,30 @@
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
       <c r="E8" s="38"/>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="30">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="32">
         <v>1.8245990000000001</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="32"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="34"/>
     </row>
     <row r="9" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
@@ -2094,14 +2194,30 @@
       <c r="M10" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="13"/>
+      <c r="N10" s="12">
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="O10" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="R10" s="12">
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="S10" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="T10" s="1">
+        <v>1</v>
+      </c>
+      <c r="U10" s="13" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
@@ -2135,14 +2251,30 @@
       <c r="M11" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="N11" s="12"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="13"/>
+      <c r="N11" s="12">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="P11" s="1">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="R11" s="12">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="S11" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="T11" s="1">
+        <v>13</v>
+      </c>
+      <c r="U11" s="13" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
@@ -2176,14 +2308,30 @@
       <c r="M12" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="N12" s="12"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="13"/>
+      <c r="N12" s="12">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="P12" s="1">
+        <v>44</v>
+      </c>
+      <c r="Q12" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="R12" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="S12" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="T12" s="1">
+        <v>44</v>
+      </c>
+      <c r="U12" s="13" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
@@ -2217,14 +2365,30 @@
       <c r="M13" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="N13" s="12"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="13"/>
+      <c r="N13" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="O13" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="P13" s="1">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="R13" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="S13" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="T13" s="1">
+        <v>45</v>
+      </c>
+      <c r="U13" s="13" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="14" spans="1:21" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
@@ -2258,14 +2422,30 @@
       <c r="M14" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="N14" s="12"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="13"/>
+      <c r="N14" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="P14" s="1">
+        <v>28</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="R14" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="S14" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="T14" s="1">
+        <v>28</v>
+      </c>
+      <c r="U14" s="13" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="15" spans="1:21" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="19" t="s">
@@ -2299,14 +2479,30 @@
       <c r="M15" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="15"/>
+      <c r="N15" s="14">
+        <v>0</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="P15" s="8">
+        <v>26</v>
+      </c>
+      <c r="Q15" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="R15" s="14">
+        <v>0</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="T15" s="8">
+        <v>26</v>
+      </c>
+      <c r="U15" s="15" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:21" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F16" s="24">
@@ -2330,6 +2526,17 @@
       <c r="L16" s="26"/>
       <c r="M16" s="27" t="s">
         <v>98</v>
+      </c>
+      <c r="N16" s="24">
+        <f>SUM(N10:N15)</f>
+        <v>1</v>
+      </c>
+      <c r="O16" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="25" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="10:13" x14ac:dyDescent="0.35">
@@ -2354,12 +2561,22 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="J18:M20"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="J4:M4"/>
@@ -2369,27 +2586,17 @@
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="J7:M7"/>
     <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="R8:U8"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="R6:U6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="J18:M20"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Reduction for K3
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Parallel-Computing-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C74BFD7-238D-4D3E-A14F-61CF64BC19EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E16953-10BD-4D91-A903-F32144EA63F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="150">
   <si>
     <t>gpu_3.cu</t>
   </si>
@@ -499,13 +499,61 @@
   </si>
   <si>
     <t>1.652984s</t>
+  </si>
+  <si>
+    <t>gpu_3_stream_0_sihouette_2_mul_1.cu</t>
+  </si>
+  <si>
+    <t>Thread 0 adds score for all its elements in the same block</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.942782 sec</t>
+  </si>
+  <si>
+    <t>1.94212s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">383.28us </t>
+  </si>
+  <si>
+    <t>4.9827ms</t>
+  </si>
+  <si>
+    <t>42.011us</t>
+  </si>
+  <si>
+    <t>1.8485ms</t>
+  </si>
+  <si>
+    <t>8.4290us</t>
+  </si>
+  <si>
+    <t>379.33us</t>
+  </si>
+  <si>
+    <t>176.35us</t>
+  </si>
+  <si>
+    <t>6.2980us</t>
+  </si>
+  <si>
+    <t>25.151us</t>
+  </si>
+  <si>
+    <t>967ns</t>
+  </si>
+  <si>
+    <t>gpu_3_stream_0_sihouette_2_mul_2.cu</t>
+  </si>
+  <si>
+    <t>Reduction sum for k3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +595,12 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -868,7 +922,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -957,19 +1011,19 @@
     <xf numFmtId="10" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -986,6 +1040,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,33 +1367,33 @@
       <c r="B2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="30" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="31"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="30" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="30" t="s">
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="31"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
@@ -1345,30 +1405,30 @@
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="32" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="32" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="32" t="s">
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="34"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
@@ -1378,30 +1438,30 @@
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
       <c r="E4" s="38"/>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="32" t="s">
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="32" t="s">
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="32" t="s">
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="34"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="32"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
@@ -1413,30 +1473,30 @@
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
       <c r="E5" s="38"/>
-      <c r="F5" s="32">
+      <c r="F5" s="30">
         <v>14</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="32">
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="30">
         <v>14</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="32">
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="30">
         <v>14</v>
       </c>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="32">
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="30">
         <v>14</v>
       </c>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="34"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="32"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
@@ -1448,30 +1508,30 @@
       <c r="C6" s="37"/>
       <c r="D6" s="37"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="32">
+      <c r="F6" s="30">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="32">
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="30">
         <v>0.04</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="32">
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="30">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="32">
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="30">
         <v>0.05</v>
       </c>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="34"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="32"/>
     </row>
     <row r="7" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
@@ -1815,6 +1875,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -1830,16 +1900,6 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1847,11 +1907,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6EC81A-94A0-466F-8869-78A7FD8B6882}">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1877,41 +1937,57 @@
     <col min="19" max="19" width="14.08984375" customWidth="1"/>
     <col min="20" max="20" width="14.81640625" customWidth="1"/>
     <col min="21" max="21" width="19.54296875" customWidth="1"/>
+    <col min="22" max="22" width="16" customWidth="1"/>
+    <col min="23" max="23" width="14.08984375" customWidth="1"/>
+    <col min="24" max="24" width="14.81640625" customWidth="1"/>
+    <col min="25" max="25" width="19.54296875" customWidth="1"/>
+    <col min="26" max="26" width="16" customWidth="1"/>
+    <col min="27" max="27" width="14.08984375" customWidth="1"/>
+    <col min="28" max="28" width="14.81640625" customWidth="1"/>
+    <col min="29" max="29" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="30" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="30" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="31"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="34"/>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
@@ -1919,32 +1995,44 @@
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="32" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="32" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="32" t="s">
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="34"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="32"/>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
@@ -1952,129 +2040,177 @@
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
       <c r="E4" s="38"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="32" t="s">
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="32" t="s">
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="32" t="s">
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="34"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
+      <c r="AC4" s="32"/>
     </row>
-    <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="32">
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="30">
         <v>42</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="32">
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="30">
         <v>42</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="32">
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="30">
         <v>42</v>
       </c>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="32">
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="30">
         <v>42</v>
       </c>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="34"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="30">
+        <v>42</v>
+      </c>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="30">
+        <v>42</v>
+      </c>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+      <c r="AC5" s="32"/>
     </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="32">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="30">
         <v>13</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="32">
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="30">
         <v>13</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="32">
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="30">
         <v>32</v>
       </c>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="34"/>
-      <c r="R6" s="32">
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="30">
         <v>13</v>
       </c>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="34"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="30">
+        <v>13</v>
+      </c>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="30">
+        <v>13</v>
+      </c>
+      <c r="AA6" s="31"/>
+      <c r="AB6" s="31"/>
+      <c r="AC6" s="32"/>
     </row>
-    <row r="7" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="32">
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="30">
         <v>0.61830700000000005</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="32">
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="30">
         <v>0.61830700000000005</v>
       </c>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="32">
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="30">
         <v>0.61830700000000005</v>
       </c>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="32">
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="30">
         <v>0.61830700000000005</v>
       </c>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33"/>
-      <c r="U7" s="34"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="30">
+        <v>0.61830700000000005</v>
+      </c>
+      <c r="W7" s="31"/>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="30">
+        <v>0.61830700000000005</v>
+      </c>
+      <c r="AA7" s="31"/>
+      <c r="AB7" s="31"/>
+      <c r="AC7" s="32"/>
     </row>
-    <row r="8" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
@@ -2082,32 +2218,42 @@
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
       <c r="E8" s="38"/>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="32">
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="30">
         <v>1.8245990000000001</v>
       </c>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="32" t="s">
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="32" t="s">
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="S8" s="33"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="34"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
+      <c r="AC8" s="32"/>
     </row>
-    <row r="9" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -2161,8 +2307,32 @@
       <c r="U9" s="11" t="s">
         <v>13</v>
       </c>
+      <c r="V9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="X9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC9" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>68</v>
       </c>
@@ -2218,8 +2388,32 @@
       <c r="U10" s="13" t="s">
         <v>107</v>
       </c>
+      <c r="V10" s="12">
+        <v>0.99619999999999997</v>
+      </c>
+      <c r="W10" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="X10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>0.99619999999999997</v>
+      </c>
+      <c r="AA10" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="40" t="s">
+        <v>137</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>5</v>
       </c>
@@ -2275,8 +2469,32 @@
       <c r="U11" s="13" t="s">
         <v>108</v>
       </c>
+      <c r="V11" s="12">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="W11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="X11" s="1">
+        <v>13</v>
+      </c>
+      <c r="Y11" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z11" s="12">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="AA11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>13</v>
+      </c>
+      <c r="AC11" s="13" t="s">
+        <v>138</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>6</v>
       </c>
@@ -2332,8 +2550,32 @@
       <c r="U12" s="13" t="s">
         <v>110</v>
       </c>
+      <c r="V12" s="12">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="W12" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="X12" s="1">
+        <v>44</v>
+      </c>
+      <c r="Y12" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z12" s="12">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AA12" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>44</v>
+      </c>
+      <c r="AC12" s="13" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>7</v>
       </c>
@@ -2389,8 +2631,32 @@
       <c r="U13" s="13" t="s">
         <v>112</v>
       </c>
+      <c r="V13" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="W13" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="X13" s="1">
+        <v>45</v>
+      </c>
+      <c r="Y13" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z13" s="12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AA13" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>45</v>
+      </c>
+      <c r="AC13" s="13" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>8</v>
       </c>
@@ -2446,8 +2712,32 @@
       <c r="U14" s="13" t="s">
         <v>114</v>
       </c>
+      <c r="V14" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="W14" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="X14" s="1">
+        <v>28</v>
+      </c>
+      <c r="Y14" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z14" s="12">
+        <v>1E-4</v>
+      </c>
+      <c r="AA14" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>28</v>
+      </c>
+      <c r="AC14" s="41" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="15" spans="1:21" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:29" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="19" t="s">
         <v>27</v>
       </c>
@@ -2503,8 +2793,32 @@
       <c r="U15" s="15" t="s">
         <v>117</v>
       </c>
+      <c r="V15" s="14">
+        <v>0</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="X15" s="8">
+        <v>26</v>
+      </c>
+      <c r="Y15" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z15" s="14">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>26</v>
+      </c>
+      <c r="AC15" s="15" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="16" spans="1:21" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:29" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F16" s="24">
         <f>SUM(F10:F15)</f>
         <v>0.99990000000000001</v>
@@ -2560,43 +2874,57 @@
       <c r="M20" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="50">
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="J18:M20"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
     <mergeCell ref="R7:U7"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="R5:U5"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="J7:M7"/>
     <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="R8:U8"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="J18:M20"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N8:Q8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Still workong on gpu_3_stream_0_sihouette_3.cu
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Parallel-Computing-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E16953-10BD-4D91-A903-F32144EA63F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017E2B39-83AD-4974-8524-FADCF0BDB875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="164">
   <si>
     <t>gpu_3.cu</t>
   </si>
@@ -547,6 +547,48 @@
   </si>
   <si>
     <t>Reduction sum for k3</t>
+  </si>
+  <si>
+    <t>1.95486s</t>
+  </si>
+  <si>
+    <t>0.25% 4.9819ms 13 383.23us</t>
+  </si>
+  <si>
+    <t>383.23us</t>
+  </si>
+  <si>
+    <t>4.9819ms</t>
+  </si>
+  <si>
+    <t>1.957022 sec [Worse Due to small no of threads per block]</t>
+  </si>
+  <si>
+    <t>42.199us</t>
+  </si>
+  <si>
+    <t>1.8568ms</t>
+  </si>
+  <si>
+    <t>8.4320us</t>
+  </si>
+  <si>
+    <t>379.45us</t>
+  </si>
+  <si>
+    <t>5.2440us</t>
+  </si>
+  <si>
+    <t>146.85us</t>
+  </si>
+  <si>
+    <t>1.0220us</t>
+  </si>
+  <si>
+    <t>26.591us</t>
+  </si>
+  <si>
+    <t>gpu_3_stream_0_sihouette_3.cu</t>
   </si>
 </sst>
 </file>
@@ -604,7 +646,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,6 +701,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -922,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1011,6 +1059,18 @@
     <xf numFmtId="10" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1018,12 +1078,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1041,10 +1095,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1364,174 +1421,174 @@
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="33" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="35" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="33" t="s">
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="33" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="34"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="33"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="30" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30" t="s">
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="30" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="30" t="s">
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="32"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="36"/>
     </row>
     <row r="4" spans="1:21" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="30" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="30" t="s">
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="30" t="s">
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="32"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="36"/>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="38">
         <v>10</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="30">
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="34">
         <v>14</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="30">
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="34">
         <v>14</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="30">
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="34">
         <v>14</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="30">
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="34">
         <v>14</v>
       </c>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="32"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="36"/>
     </row>
     <row r="6" spans="1:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="38">
         <v>0.32800000000000001</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="30">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="34">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="30">
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="34">
         <v>0.04</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="30">
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="34">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="30">
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="34">
         <v>0.05</v>
       </c>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="32"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="36"/>
     </row>
     <row r="7" spans="1:21" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
@@ -1875,16 +1932,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
@@ -1900,6 +1947,16 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1909,9 +1966,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6EC81A-94A0-466F-8869-78A7FD8B6882}">
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="59" zoomScaleNormal="50" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1952,306 +2009,308 @@
       <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="33" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="33" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="34"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="33"/>
     </row>
     <row r="3" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="30" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30" t="s">
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="30" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="30" t="s">
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="30" t="s">
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="36"/>
+      <c r="V3" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="W3" s="31"/>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="30" t="s">
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="AA3" s="31"/>
-      <c r="AB3" s="31"/>
-      <c r="AC3" s="32"/>
+      <c r="AA3" s="35"/>
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="36"/>
     </row>
     <row r="4" spans="1:29" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="30" t="s">
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="30" t="s">
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="30" t="s">
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="30" t="s">
+      <c r="W4" s="35"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="AA4" s="31"/>
-      <c r="AB4" s="31"/>
-      <c r="AC4" s="32"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="36"/>
     </row>
     <row r="5" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30">
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="34">
         <v>42</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="30">
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="34">
         <v>42</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="30">
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="34">
         <v>42</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="30">
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="36"/>
+      <c r="R5" s="34">
         <v>42</v>
       </c>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="32"/>
-      <c r="V5" s="30">
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="36"/>
+      <c r="V5" s="34">
         <v>42</v>
       </c>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="30">
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="36"/>
+      <c r="Z5" s="34">
         <v>42</v>
       </c>
-      <c r="AA5" s="31"/>
-      <c r="AB5" s="31"/>
-      <c r="AC5" s="32"/>
+      <c r="AA5" s="35"/>
+      <c r="AB5" s="35"/>
+      <c r="AC5" s="36"/>
     </row>
     <row r="6" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30">
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="34">
         <v>13</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="30">
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="34">
         <v>13</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="30">
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="34">
         <v>32</v>
       </c>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="30">
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="34">
         <v>13</v>
       </c>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="30">
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="34">
         <v>13</v>
       </c>
-      <c r="W6" s="31"/>
-      <c r="X6" s="31"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="30">
+      <c r="W6" s="35"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="34">
         <v>13</v>
       </c>
-      <c r="AA6" s="31"/>
-      <c r="AB6" s="31"/>
-      <c r="AC6" s="32"/>
+      <c r="AA6" s="35"/>
+      <c r="AB6" s="35"/>
+      <c r="AC6" s="36"/>
     </row>
     <row r="7" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="30">
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="34">
         <v>0.61830700000000005</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="30">
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="34">
         <v>0.61830700000000005</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="30">
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="34">
         <v>0.61830700000000005</v>
       </c>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="30">
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="34">
         <v>0.61830700000000005</v>
       </c>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="30">
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="34">
         <v>0.61830700000000005</v>
       </c>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="30">
+      <c r="W7" s="35"/>
+      <c r="X7" s="35"/>
+      <c r="Y7" s="36"/>
+      <c r="Z7" s="34">
         <v>0.61830700000000005</v>
       </c>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="32"/>
+      <c r="AA7" s="35"/>
+      <c r="AB7" s="35"/>
+      <c r="AC7" s="36"/>
     </row>
     <row r="8" spans="1:29" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="30" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="30">
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="34">
         <v>1.8245990000000001</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="30" t="s">
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="30" t="s">
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="30" t="s">
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="W8" s="31"/>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="32"/>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="31"/>
-      <c r="AB8" s="31"/>
-      <c r="AC8" s="32"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="36"/>
+      <c r="Z8" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA8" s="43"/>
+      <c r="AB8" s="43"/>
+      <c r="AC8" s="44"/>
     </row>
     <row r="9" spans="1:29" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
@@ -2397,20 +2456,20 @@
       <c r="X10" s="1">
         <v>1</v>
       </c>
-      <c r="Y10" s="40" t="s">
+      <c r="Y10" s="30" t="s">
         <v>137</v>
       </c>
       <c r="Z10" s="12">
         <v>0.99619999999999997</v>
       </c>
       <c r="AA10" s="23" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="AB10" s="1">
         <v>1</v>
       </c>
-      <c r="AC10" s="40" t="s">
-        <v>137</v>
+      <c r="AC10" s="30" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.35">
@@ -2481,17 +2540,17 @@
       <c r="Y11" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="Z11" s="12">
-        <v>2.5999999999999999E-3</v>
+      <c r="Z11" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="AA11" s="23" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="AB11" s="1">
         <v>13</v>
       </c>
       <c r="AC11" s="13" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.35">
@@ -2566,13 +2625,13 @@
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="AA12" s="23" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="AB12" s="1">
         <v>44</v>
       </c>
       <c r="AC12" s="13" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.35">
@@ -2647,13 +2706,13 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="AA13" s="23" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="AB13" s="1">
         <v>45</v>
       </c>
       <c r="AC13" s="13" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:29" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
@@ -2721,20 +2780,20 @@
       <c r="X14" s="1">
         <v>28</v>
       </c>
-      <c r="Y14" s="41" t="s">
+      <c r="Y14" s="31" t="s">
         <v>145</v>
       </c>
       <c r="Z14" s="12">
         <v>1E-4</v>
       </c>
       <c r="AA14" s="23" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="AB14" s="1">
         <v>28</v>
       </c>
-      <c r="AC14" s="41" t="s">
-        <v>145</v>
+      <c r="AC14" s="31" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2809,13 +2868,13 @@
         <v>0</v>
       </c>
       <c r="AA15" s="7" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="AB15" s="8">
         <v>26</v>
       </c>
       <c r="AC15" s="15" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2853,28 +2912,73 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J18" s="39" t="s">
+    <row r="17" spans="10:17" x14ac:dyDescent="0.35">
+      <c r="N17" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="36"/>
+    </row>
+    <row r="18" spans="10:17" x14ac:dyDescent="0.35">
+      <c r="J18" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
     </row>
-    <row r="19" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
+    <row r="19" spans="10:17" x14ac:dyDescent="0.35">
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
     </row>
-    <row r="20" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
+    <row r="20" spans="10:17" x14ac:dyDescent="0.35">
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="51">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="J18:M20"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="N17:Q17"/>
     <mergeCell ref="V7:Y7"/>
     <mergeCell ref="V8:Y8"/>
     <mergeCell ref="Z2:AC2"/>
@@ -2889,42 +2993,6 @@
     <mergeCell ref="V4:Y4"/>
     <mergeCell ref="V5:Y5"/>
     <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="J18:M20"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="R8:U8"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="N7:Q7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>